<commit_message>
mise à jour connexion BdD avec ID en ligne
</commit_message>
<xml_diff>
--- a/Analyse/dictionnaire de données.xlsx
+++ b/Analyse/dictionnaire de données.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="68">
   <si>
     <t>Nom de la colonne</t>
   </si>
@@ -149,13 +149,82 @@
   </si>
   <si>
     <t>Profil_joueur</t>
+  </si>
+  <si>
+    <t>Recherche</t>
+  </si>
+  <si>
+    <t>id-pmessage</t>
+  </si>
+  <si>
+    <t>Identifiant unique du message privé</t>
+  </si>
+  <si>
+    <t>Identifiant de l'utilisateur émetteur</t>
+  </si>
+  <si>
+    <t>Identifiant du profil du destinataire</t>
+  </si>
+  <si>
+    <t>contenu</t>
+  </si>
+  <si>
+    <t>Contenu du message privé</t>
+  </si>
+  <si>
+    <t>Table_de_jeu</t>
+  </si>
+  <si>
+    <t>id-tablechat</t>
+  </si>
+  <si>
+    <t>Identifiant unique du chat de table</t>
+  </si>
+  <si>
+    <t>id-table</t>
+  </si>
+  <si>
+    <t>Identifiant de la table associée</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>Contenu du message dans le chat</t>
+  </si>
+  <si>
+    <t>id-message</t>
+  </si>
+  <si>
+    <t>Identifiant unique du message</t>
+  </si>
+  <si>
+    <t>Contenu du message</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>DATETIME</t>
+  </si>
+  <si>
+    <t>Date et heure d'envoi du message</t>
+  </si>
+  <si>
+    <t>chat</t>
+  </si>
+  <si>
+    <t>Dictionnaire de données</t>
+  </si>
+  <si>
+    <t>Dictionnaire des données</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +240,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -180,7 +273,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -188,21 +281,244 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:N13"/>
+  <dimension ref="D1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28:F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -521,241 +837,804 @@
     <col min="8" max="8" width="18.88671875" customWidth="1"/>
     <col min="9" max="9" width="12.44140625" customWidth="1"/>
     <col min="10" max="10" width="33.5546875" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" customWidth="1"/>
+    <col min="14" max="14" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D1" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+    </row>
+    <row r="2" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" spans="4:10" ht="18" x14ac:dyDescent="0.3">
+      <c r="D3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13"/>
+      <c r="H3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="12"/>
+      <c r="J3" s="13"/>
+    </row>
+    <row r="4" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="H4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="4:14" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="J4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="4:14" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="2" t="s">
+    </row>
+    <row r="5" spans="4:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="4:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="E6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="4:14" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="2" t="s">
-        <v>6</v>
+        <v>25</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="4:10" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>3</v>
+      <c r="F7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="4:14" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="4:10" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>27</v>
+      <c r="F8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="4:14" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="2" t="s">
-        <v>11</v>
+      <c r="J8" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="4:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="4:10" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="4:14" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="4:10" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="4:14" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>33</v>
+      <c r="F11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="4:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="4:10" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="4:10" ht="18" x14ac:dyDescent="0.3">
+      <c r="D14" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="13"/>
+      <c r="H14" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" s="12"/>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D17" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="4:10" ht="18" x14ac:dyDescent="0.3">
+      <c r="D20" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="13"/>
+      <c r="H20" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="I20" s="15"/>
+      <c r="J20" s="16"/>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D22" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D23" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D24" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="4:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="4:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="19"/>
+      <c r="F28" s="20"/>
+    </row>
+    <row r="29" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D29" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D33" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D34" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D35" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D36" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D37" s="21"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="22"/>
+    </row>
+    <row r="38" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D38" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D39" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D40" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D41" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D42" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D43" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F43" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="4:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="2" t="s">
+    <row r="44" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D44" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="F44" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="4:14" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="2" t="s">
+    <row r="45" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D45" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="E45" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="F45" s="6" t="s">
         <v>40</v>
       </c>
     </row>
+    <row r="46" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D46" s="21"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="22"/>
+    </row>
+    <row r="47" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D47" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D48" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D49" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D50" s="21"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="22"/>
+    </row>
+    <row r="51" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D51" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D52" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D53" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D54" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D55" s="21"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="22"/>
+    </row>
+    <row r="56" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D56" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D57" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D58" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="59" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D59" s="21"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="22"/>
+    </row>
+    <row r="60" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D60" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D61" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="62" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D62" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="63" spans="4:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D63" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="H4:J4"/>
+  <mergeCells count="8">
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D1:J2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>